<commit_message>
Add region code to xlsx file
</commit_message>
<xml_diff>
--- a/data/Populations_USA.xlsx
+++ b/data/Populations_USA.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18492" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21780" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
   <si>
     <t>Total</t>
   </si>
@@ -172,16 +177,182 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,14 +375,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,1421 +686,1587 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1">
+    <row r="1" spans="1:9">
+      <c r="C1">
         <v>1990</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2000</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2010</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2015</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2020</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2030</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>2040</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>248709873</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>281421906</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>308745538</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>321418820</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>332527547.99389899</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>357975718.83859098</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>379392778.54187202</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>4040587</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>4447100</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>4779735</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>4858979</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>4911277.6891100593</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>5029832.515944778</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>5056796.4572937628</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>550043</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>626932</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>710231</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>738432</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>751328.12837596238</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>792187.75583763805</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>819954.05513561098</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>3665228</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>5130632</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>6329013</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>6828065</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>7268693.6504087653</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>8238407.360113332</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>9166279.060121052</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>2350725</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>2673400</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>2915921</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>2978204</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>3038491.345688663</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>3155797.6897252733</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>3217534.5514366431</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>29760021</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>33871648</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>37253956</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>39144818</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>40438639.916706286</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>43751116.139102437</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>46467001.490301341</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>3294394</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>4301261</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>5029196</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>5456574</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>5843359.3191798776</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>6766982.8721162789</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>7692906.9059937485</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>3287116</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>3405565</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>3574097</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>3590886</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>3593541.8573748656</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>3601202.4259101767</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>3542707.3258033688</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>666168</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>783600</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>897934</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>945934</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>987393.11397790629</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>1082191.7661196284</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>1164343.8981806587</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
         <v>606900</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>572059</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>601723</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>672228</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>732551.99412044312</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>888891.49529709667</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>1058819.5762361488</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>12937926</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>15982378</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>18801311</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>20271272</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>21877256.722615965</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>25372664.05942804</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>28886983.32355551</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>6478216</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>8186453</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>9687653</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>10214860</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>10725350.805434817</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>11835126.133303933</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>12820270.562845577</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>1108229</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>1211537</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>1360301</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>1431603</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>1453902.3499037491</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>1548830.5735724412</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>1619703.4324594336</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>1006749</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>1293953</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>1567582</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>1654930</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>1777249.2925173524</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>2008329.1196092044</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>2227841.7366631152</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>11430602</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>12419293</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>12830632</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>12859995</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>12791188.005270034</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>12709901.030032199</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>12397564.33019612</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>5544159</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>6080485</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>6483800</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>6619680</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>6737581.4314494021</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>6978253.8454271313</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>7095000.250901836</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>2776755</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>2926324</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>3046350</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>3123899</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>3184239.7976254108</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>3317412.4775014794</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>3392783.1048486815</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>2477574</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>2688418</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>2853118</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>2911641</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>2936212.2204559683</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>3011782.4847691092</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>3032652.715673198</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>3685296</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>4041769</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>4339362</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>4425092</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>4498532.6538571361</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>4648189.5061446279</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>4714761.0784620559</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <v>4219973</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>4468976</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>4515770</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>4649676</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>4742900.1566064348</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>4945783.0300401971</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>5062779.9671766628</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>1227928</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>1274923</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>1328361</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>1329328</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>1338780.4762898579</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>1344841.4228721661</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>1326159.3139775181</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>4781468</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>5296486</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>5773552</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>6006401</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>6161345.3109492073</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>6553547.7843522374</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>6842901.7827909803</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24" s="1">
         <v>6016425</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>6349097</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>6547629</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>6794422</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>6982092.0707958555</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>7420882.114077759</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>7742628.2694238983</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="1">
         <v>9295297</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>9938444</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>9883635</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>9922576</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>9992315.2647452652</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>10068940.875305697</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>9960115.3633058406</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="1">
         <v>4375099</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>4919479</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>5303925</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>5489594</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>5683665.7455427563</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>6070551.3562471187</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>6364886.4612853369</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="1">
         <v>2573216</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>2844658</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>2967297</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>2992333</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>2990498.4134555459</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>3003963.0644783387</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>2962160.0182121778</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28" s="1">
         <v>5117073</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>5595211</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>5988927</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>6083672</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>6161471.2561612437</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>6318126.069965167</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>6359969.9439152488</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
+      <c r="C29" s="1">
         <v>799065</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>902195</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>989415</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>1032949</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>1074634.5451293329</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>1163353.1164727476</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>1236303.8825375126</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="1">
+      <c r="C30" s="1">
         <v>1578385</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>1711263</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>1826341</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>1896190</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>1956876.0482607689</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>2089840.8770083492</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>2190917.5635631573</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31" s="1">
         <v>1201833</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>1998257</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>2700551</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>2890845</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>3119264.7552559385</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>3591042.5094382935</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>4058371.2189145912</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C32" s="1">
         <v>1109252</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>1235786</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>1316472</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>1330608</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>1352917.485551331</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>1385798.5611408385</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>1393451.3721175529</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33" s="1">
         <v>7730188</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>8414350</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>8791894</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>8958013</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>9088074.2435212396</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>9363317.3358545341</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>9470012.0989358611</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="1">
+      <c r="C34" s="1">
         <v>1515069</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>1819046</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>2059180</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>2085109</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>2099134.3861752246</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>2132823.1135228886</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <v>2127317.6794886789</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="1">
+      <c r="C35" s="1">
         <v>17990455</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>18976457</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>19378104</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>19795791</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>20031150.391204506</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>20638066.090743259</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>20873487.750148162</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="1">
+      <c r="C36" s="1">
         <v>6628637</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>8049313</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>9535475</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>10042802</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>10568032.768898655</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>11673848.679962793</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <v>12658926.638546815</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="1">
+      <c r="C37" s="1">
         <v>638800</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>642200</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>672591</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>756927</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>789402.5154641401</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>923452.18559182948</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <v>1060457.4225212268</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="1">
+      <c r="C38" s="1">
         <v>10847115</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>11353140</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>11536502</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>11613423</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>11705262.032378284</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>11837405.16462896</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <v>11751540.464269064</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="1">
+      <c r="C39" s="1">
         <v>3145585</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>3450654</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>3751354</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <v>3911338</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="1">
         <v>4001180.4541401593</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>4253603.7393453438</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>4439037.7136998521</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="1">
+      <c r="C40" s="1">
         <v>2842321</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>3421399</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>3831074</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>4028977</v>
       </c>
-      <c r="F40" s="1">
+      <c r="G40" s="1">
         <v>4267533.7999668987</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
         <v>4738074.1333143422</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <v>5164040.6080865115</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="1">
+      <c r="C41" s="1">
         <v>11881643</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>12281054</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>12702379</v>
       </c>
-      <c r="E41" s="1">
+      <c r="F41" s="1">
         <v>12802503</v>
       </c>
-      <c r="F41" s="1">
+      <c r="G41" s="1">
         <v>12844884.682541594</v>
       </c>
-      <c r="G41" s="1">
+      <c r="H41" s="1">
         <v>12946244.536413312</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <v>12809150.178074736</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="1">
+      <c r="C42" s="1">
         <v>1003464</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>1048319</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>1052567</v>
       </c>
-      <c r="E42" s="1">
+      <c r="F42" s="1">
         <v>1056298</v>
       </c>
-      <c r="F42" s="1">
+      <c r="G42" s="1">
         <v>1062333.8952496243</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <v>1068663.0174351365</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <v>1055318.2224670723</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="1">
+      <c r="C43" s="1">
         <v>3486703</v>
       </c>
-      <c r="C43" s="1">
+      <c r="D43" s="1">
         <v>4012012</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>4625364</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>4896146</v>
       </c>
-      <c r="F43" s="1">
+      <c r="G43" s="1">
         <v>5184564.4374957969</v>
       </c>
-      <c r="G43" s="1">
+      <c r="H43" s="1">
         <v>5792247.2299281713</v>
       </c>
-      <c r="H43" s="1">
+      <c r="I43" s="1">
         <v>6352502.134922483</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="1">
+      <c r="C44" s="1">
         <v>696004</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D44" s="1">
         <v>754844</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <v>814180</v>
       </c>
-      <c r="E44" s="1">
+      <c r="F44" s="1">
         <v>858469</v>
       </c>
-      <c r="F44" s="1">
+      <c r="G44" s="1">
         <v>891688.01332649647</v>
       </c>
-      <c r="G44" s="1">
+      <c r="H44" s="1">
         <v>973360.86404684361</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <v>1043032.2762363398</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="1">
+      <c r="C45" s="1">
         <v>4877185</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="1">
         <v>5689283</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>6346110</v>
       </c>
-      <c r="E45" s="1">
+      <c r="F45" s="1">
         <v>6600299</v>
       </c>
-      <c r="F45" s="1">
+      <c r="G45" s="1">
         <v>6861855.9604063192</v>
       </c>
-      <c r="G45" s="1">
+      <c r="H45" s="1">
         <v>7395105.8485040888</v>
       </c>
-      <c r="H45" s="1">
+      <c r="I45" s="1">
         <v>7823662.4911053712</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="1">
+      <c r="C46" s="1">
         <v>16986510</v>
       </c>
-      <c r="C46" s="1">
+      <c r="D46" s="1">
         <v>20851820</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>25145561</v>
       </c>
-      <c r="E46" s="1">
+      <c r="F46" s="1">
         <v>27469114</v>
       </c>
-      <c r="F46" s="1">
+      <c r="G46" s="1">
         <v>29604099.489181209</v>
       </c>
-      <c r="G46" s="1">
+      <c r="H46" s="1">
         <v>34738481.792648926</v>
       </c>
-      <c r="H46" s="1">
+      <c r="I46" s="1">
         <v>40015912.841135815</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="1">
+      <c r="C47" s="1">
         <v>1722850</v>
       </c>
-      <c r="C47" s="1">
+      <c r="D47" s="1">
         <v>2233169</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>2763885</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <v>2995919</v>
       </c>
-      <c r="F47" s="1">
+      <c r="G47" s="1">
         <v>3240568.9753061314</v>
       </c>
-      <c r="G47" s="1">
+      <c r="H47" s="1">
         <v>3786962.6692582713</v>
       </c>
-      <c r="H47" s="1">
+      <c r="I47" s="1">
         <v>4344338.8632934</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="1">
+      <c r="C48" s="1">
         <v>562758</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D48" s="1">
         <v>608827</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>625741</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="1">
         <v>626042</v>
       </c>
-      <c r="F48" s="1">
+      <c r="G48" s="1">
         <v>622868.33412478375</v>
       </c>
-      <c r="G48" s="1">
+      <c r="H48" s="1">
         <v>617968.51149770047</v>
       </c>
-      <c r="H48" s="1">
+      <c r="I48" s="1">
         <v>601865.36934048962</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="1">
+      <c r="C49" s="1">
         <v>6187358</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>7078515</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>8001024</v>
       </c>
-      <c r="E49" s="1">
+      <c r="F49" s="1">
         <v>8382993</v>
       </c>
-      <c r="F49" s="1">
+      <c r="G49" s="1">
         <v>8655021.3267997373</v>
       </c>
-      <c r="G49" s="1">
+      <c r="H49" s="1">
         <v>9331665.5438315067</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <v>9876728.2012210898</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="1">
+      <c r="C50" s="1">
         <v>4866692</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D50" s="1">
         <v>5894121</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>6724540</v>
       </c>
-      <c r="E50" s="1">
+      <c r="F50" s="1">
         <v>7170351</v>
       </c>
-      <c r="F50" s="1">
+      <c r="G50" s="1">
         <v>7681818.4170901598</v>
       </c>
-      <c r="G50" s="1">
+      <c r="H50" s="1">
         <v>8746492.8647534549</v>
       </c>
-      <c r="H50" s="1">
+      <c r="I50" s="1">
         <v>9776125.5521557163</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="1">
+      <c r="C51" s="1">
         <v>1793477</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>1808344</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>1852996</v>
       </c>
-      <c r="E51" s="1">
+      <c r="F51" s="1">
         <v>1844128</v>
       </c>
-      <c r="F51" s="1">
+      <c r="G51" s="1">
         <v>1801966.0658414897</v>
       </c>
-      <c r="G51" s="1">
+      <c r="H51" s="1">
         <v>1746576.677428741</v>
       </c>
-      <c r="H51" s="1">
+      <c r="I51" s="1">
         <v>1661849.2298883353</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="1">
+      <c r="C52" s="1">
         <v>4891769</v>
       </c>
-      <c r="C52" s="1">
+      <c r="D52" s="1">
         <v>5363675</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>5686986</v>
       </c>
-      <c r="E52" s="1">
+      <c r="F52" s="1">
         <v>5771337</v>
       </c>
-      <c r="F52" s="1">
+      <c r="G52" s="1">
         <v>5837176.3904889319</v>
       </c>
-      <c r="G52" s="1">
+      <c r="H52" s="1">
         <v>5971616.7644396629</v>
       </c>
-      <c r="H52" s="1">
+      <c r="I52" s="1">
         <v>5997136.7936651846</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="1">
+      <c r="C53" s="1">
         <v>453588</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>493782</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>563626</v>
       </c>
-      <c r="E53" s="1">
+      <c r="F53" s="1">
         <v>586107</v>
       </c>
-      <c r="F53" s="1">
+      <c r="G53" s="1">
         <v>585379.59148167947</v>
       </c>
-      <c r="G53" s="1">
+      <c r="H53" s="1">
         <v>605972.0440876506</v>
       </c>
-      <c r="H53" s="1">
+      <c r="I53" s="1">
         <v>615786.99934104551</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>